<commit_message>
added edge sensor code
</commit_message>
<xml_diff>
--- a/STM32-ROMI-Pin_List_Rev_A.xlsx
+++ b/STM32-ROMI-Pin_List_Rev_A.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\STM32-ROMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63E4565-F2A2-435B-9886-AF81984C82DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD7804-D5F4-4858-8412-1262D168DF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="1" r:id="rId1"/>
     <sheet name="Timer Map" sheetId="3" r:id="rId2"/>
-    <sheet name="Timer Calculator" sheetId="6" r:id="rId3"/>
-    <sheet name="ROMI Connectors" sheetId="2" r:id="rId4"/>
-    <sheet name="Libraries" sheetId="4" r:id="rId5"/>
-    <sheet name="I2C Map" sheetId="5" r:id="rId6"/>
+    <sheet name="Math" sheetId="7" r:id="rId3"/>
+    <sheet name="Timer Calculator" sheetId="6" r:id="rId4"/>
+    <sheet name="ROMI Connectors" sheetId="2" r:id="rId5"/>
+    <sheet name="Libraries" sheetId="4" r:id="rId6"/>
+    <sheet name="I2C Map" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="232">
   <si>
     <t>Chip Line:</t>
   </si>
@@ -659,6 +660,78 @@
   </si>
   <si>
     <t>Interupt</t>
+  </si>
+  <si>
+    <t>sample tate</t>
+  </si>
+  <si>
+    <t>HZ</t>
+  </si>
+  <si>
+    <t>Sec</t>
+  </si>
+  <si>
+    <t>Sample Period</t>
+  </si>
+  <si>
+    <t>Encoder Resolution</t>
+  </si>
+  <si>
+    <t>Gear Ratio</t>
+  </si>
+  <si>
+    <t>to 1</t>
+  </si>
+  <si>
+    <t>Counts/rev</t>
+  </si>
+  <si>
+    <t>Wheel Diameter</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Wheel Circumference</t>
+  </si>
+  <si>
+    <t>Counts/mm</t>
+  </si>
+  <si>
+    <t>MAX RPM</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>Max RPS</t>
+  </si>
+  <si>
+    <t>Max Rad/s</t>
+  </si>
+  <si>
+    <t>Max Counts per sample</t>
+  </si>
+  <si>
+    <t>Counts/rad</t>
+  </si>
+  <si>
+    <t>Enc to Rad/s</t>
+  </si>
+  <si>
+    <t>Enc/Vel</t>
+  </si>
+  <si>
+    <t>Rad/s</t>
+  </si>
+  <si>
+    <t>rps</t>
+  </si>
+  <si>
+    <t>Max Counts/Sec</t>
+  </si>
+  <si>
+    <t>1/sec</t>
   </si>
 </sst>
 </file>
@@ -5668,7 +5741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C93889-D2DC-4DAC-B58A-4E6965021699}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -6026,6 +6099,179 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A193F010-FDB0-4A2D-8148-A1705E9BF8AF}">
+  <dimension ref="B3:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4">
+        <f>1/C3</f>
+        <v>0.02</v>
+      </c>
+      <c r="D4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11">
+        <f>(C10/2)*3.1415*2</f>
+        <v>226.18800000000002</v>
+      </c>
+      <c r="D11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12">
+        <f>C8/C11</f>
+        <v>5.3053212372009124</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15">
+        <f>C14/60</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="D15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16">
+        <f>C15*6.28</f>
+        <v>13.606666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18">
+        <f>C15*C8</f>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19">
+        <f>C18*C4</f>
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67014346-00EF-47D2-B856-559F1327E32B}">
   <dimension ref="A4:D5"/>
   <sheetViews>
@@ -6074,7 +6320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221C21A2-B886-4917-974F-8AE92A61D9B0}">
   <dimension ref="A3:E6"/>
   <sheetViews>
@@ -6157,7 +6403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3FA9F3-5075-412B-8D1F-1D8165512D36}">
   <dimension ref="A3:B8"/>
   <sheetViews>
@@ -6210,7 +6456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5698921E-23DA-4026-8E32-BD7C5A45C05A}">
   <dimension ref="A2:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
working with ralph, slightly better
</commit_message>
<xml_diff>
--- a/STM32-ROMI-Pin_List_Rev_A.xlsx
+++ b/STM32-ROMI-Pin_List_Rev_A.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\STM32-ROMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD7804-D5F4-4858-8412-1262D168DF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48413A51-DC03-48AC-9E88-802F62125A83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -662,9 +662,6 @@
     <t>Interupt</t>
   </si>
   <si>
-    <t>sample tate</t>
-  </si>
-  <si>
     <t>HZ</t>
   </si>
   <si>
@@ -732,6 +729,9 @@
   </si>
   <si>
     <t>1/sec</t>
+  </si>
+  <si>
+    <t>Sample Rate</t>
   </si>
 </sst>
 </file>
@@ -6103,7 +6103,7 @@
   <dimension ref="B3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6113,30 +6113,30 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4">
         <f>1/C3</f>
         <v>0.02</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -6144,18 +6144,18 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8">
         <v>1200</v>
@@ -6163,30 +6163,30 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10">
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C11">
         <f>(C10/2)*3.1415*2</f>
         <v>226.18800000000002</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12">
         <f>C8/C11</f>
@@ -6195,30 +6195,30 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C14">
         <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15">
         <f>C14/60</f>
         <v>2.1666666666666665</v>
       </c>
       <c r="D15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16">
         <f>C15*6.28</f>
@@ -6227,7 +6227,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C18">
         <f>C15*C8</f>
@@ -6236,34 +6236,42 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19">
         <f>C18*C4</f>
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="C21">
+        <f>C8/(2*3.1415)</f>
+        <v>190.99156453923283</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="C24">
+        <f>C16/C19</f>
+        <v>0.26166666666666666</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>